<commit_message>
L.K | 05/09/2023 11:46 | Criadas as condicionais para CNPJs com nenhum processo, com apenas 1 processo e com varios processos. Atualmente rodando para todos os CNPJs.
</commit_message>
<xml_diff>
--- a/testes/teste_pre_dot - Copia.xlsx
+++ b/testes/teste_pre_dot - Copia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Área de Trabalho\a01_codigos\A00_predot_python\z_resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Área de Trabalho\a01_codigos\a16_LegalTrackHub\testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F3980F-92CF-4294-AAFD-F22DD87EA65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2E813C-C6EA-4ECB-9995-D2468B92A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D331CF9-2202-4893-9E60-6CD95649DCEB}"/>
   </bookViews>
@@ -36,23 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>nada</t>
   </si>
   <si>
-    <t>04.615.036/0001-30</t>
-  </si>
-  <si>
-    <t>40.584.562/0001-44</t>
-  </si>
-  <si>
     <t>73.965.444/0001-35</t>
   </si>
   <si>
-    <t>08.305.646/0001-99</t>
-  </si>
-  <si>
     <t>07.774.941/0001-21</t>
   </si>
   <si>
@@ -81,6 +72,9 @@
   </si>
   <si>
     <t>07.783.207/0001-29</t>
+  </si>
+  <si>
+    <t>21.578.639/0001-29</t>
   </si>
 </sst>
 </file>
@@ -432,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2B2711-19E2-495D-8661-13B9160D91DD}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,72 +441,67 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>